<commit_message>
Updated the JSON inputs
Updated the JSON inputs
</commit_message>
<xml_diff>
--- a/API_Server_Test_Case.xlsx
+++ b/API_Server_Test_Case.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MTS\One-Week-Project-SP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MTS\One-Week-Project-SP\Friend-Management-API-Server-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16BE7CC9-1F92-4719-BD8D-9CE8E5C885A2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CDE878B-4FD5-4241-BAF7-0DC8CDF8F74C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" xr2:uid="{904B0131-C46D-46F9-8EB6-358034E6D2D8}"/>
   </bookViews>
@@ -52,116 +52,116 @@
     <t>{   "error": Input has to be a valid email ID }</t>
   </si>
   <si>
+    <t xml:space="preserve">{   "success": true,   "friends" :     [       'common@example.com'     ],   "count" : 1    } </t>
+  </si>
+  <si>
+    <t>{   "error": No Common friends }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">API 4 - Subscribe to Updates
+Input
+{   "requestor": "lisa@example.com",   "target": "john@example.com" } </t>
+  </si>
+  <si>
+    <t xml:space="preserve">{   "success": true } </t>
+  </si>
+  <si>
+    <t xml:space="preserve">API 5 - Block Updates
+Input
+{   "requestor": "andy@example.com",   "target": "john@example.com" } </t>
+  </si>
+  <si>
+    <t xml:space="preserve">API 4 - Subscribe to Updates
+Input
+{   "requestor": "lisa",   "target": "john@example.com" } </t>
+  </si>
+  <si>
+    <t xml:space="preserve">{   "error": requestor has to be a valid email ID } </t>
+  </si>
+  <si>
+    <t xml:space="preserve">API 4 - Subscribe to Updates
+Input
+{   "requestor": "lisa@example.com",   "target": "john" } </t>
+  </si>
+  <si>
+    <t xml:space="preserve">{   "error": target has to be a valid email ID } </t>
+  </si>
+  <si>
+    <t xml:space="preserve">API 5 - Block Updates
+Input
+{   "requestor": "andy",   "target": "john@example.com" } </t>
+  </si>
+  <si>
+    <t xml:space="preserve">API 5 - Block Updates
+Input
+{   "requestor": "andy@example.com",   "target": "john" } </t>
+  </si>
+  <si>
+    <t xml:space="preserve">API 6 - Retrieve all email addresses that can receive updates from an email address
+Input
+{   "sender":  "john@example.com",   "text": "Hello World! kate@example.com" } </t>
+  </si>
+  <si>
+    <t xml:space="preserve">API 6 - Retrieve all email addresses that can receive updates from an email address
+Input
+{   "sender":  "john@example.com",   "text": "Hello World!" } </t>
+  </si>
+  <si>
+    <t xml:space="preserve">{   "success": true   "recipients":     [ "lisa@example.com",       "andy@example.com", "common@example.com"   ] } </t>
+  </si>
+  <si>
+    <t xml:space="preserve">{   "success": true   "recipients":     [ "lisa@example.com",       "andy@example.com", "common@example.com", "kate@example.com"    ] } </t>
+  </si>
+  <si>
+    <t>{   "error": Input has to be valid email ID }</t>
+  </si>
+  <si>
     <t xml:space="preserve">API 1 - Add friend
 Input
-{   friends:     
-[       'andy@example.com',       'john@example.com'     ] } </t>
+{   "friends":     
+[       "andy@example.com",       "john@example.com"     ] } </t>
   </si>
   <si>
     <t xml:space="preserve">API 1 - Add friend
 Input
-{   friends:     
-[       'andy',       'john'     ] } </t>
+{   "friends":     
+[       "andy",       "john"     ] } </t>
   </si>
   <si>
     <t xml:space="preserve">API 2 - Get Friend List
 Input
-{   email: 'andy@example.com' 
+{   "email": "andy@example.com" 
 } </t>
   </si>
   <si>
     <t xml:space="preserve">API 2 - Get Friend List
 Input
-{   email: 'andy' 
+{   "email": "andy"
 } </t>
   </si>
   <si>
+    <t xml:space="preserve">API 1 - Add friend
+Input
+{   "friends":     
+[       "andy@example.com",       "common@example.com"] } </t>
+  </si>
+  <si>
+    <t xml:space="preserve">API 1 - Add friend
+Input
+{   "friends":     
+[       "john@example.com",       "common@example.com"] } </t>
+  </si>
+  <si>
     <t xml:space="preserve">API 3 - Get Common Friends
 Input
-{   friends:     
-[       'andy@example.com',       'john@example.com'     ] } </t>
-  </si>
-  <si>
-    <t xml:space="preserve">API 1 - Add friend
-Input
-{   friends:     
-[       'john@example.com',       'common@example.com'] } </t>
-  </si>
-  <si>
-    <t xml:space="preserve">API 1 - Add friend
-Input
-{   friends:     
-[       'andy@example.com',       'common@example.com'] } </t>
-  </si>
-  <si>
-    <t xml:space="preserve">{   "success": true,   "friends" :     [       'common@example.com'     ],   "count" : 1    } </t>
+{   "friends":     
+[       "andy@example.com",       "john@example.com"     ] } </t>
   </si>
   <si>
     <t xml:space="preserve">API 3 - Get Common Friends
 Input
-{   friends:     
-[       'andy@example.com',       'kevin@example.com'     ] } </t>
-  </si>
-  <si>
-    <t>{   "error": No Common friends }</t>
-  </si>
-  <si>
-    <t xml:space="preserve">API 4 - Subscribe to Updates
-Input
-{   "requestor": "lisa@example.com",   "target": "john@example.com" } </t>
-  </si>
-  <si>
-    <t xml:space="preserve">{   "success": true } </t>
-  </si>
-  <si>
-    <t xml:space="preserve">API 5 - Block Updates
-Input
-{   "requestor": "andy@example.com",   "target": "john@example.com" } </t>
-  </si>
-  <si>
-    <t xml:space="preserve">API 4 - Subscribe to Updates
-Input
-{   "requestor": "lisa",   "target": "john@example.com" } </t>
-  </si>
-  <si>
-    <t xml:space="preserve">{   "error": requestor has to be a valid email ID } </t>
-  </si>
-  <si>
-    <t xml:space="preserve">API 4 - Subscribe to Updates
-Input
-{   "requestor": "lisa@example.com",   "target": "john" } </t>
-  </si>
-  <si>
-    <t xml:space="preserve">{   "error": target has to be a valid email ID } </t>
-  </si>
-  <si>
-    <t xml:space="preserve">API 5 - Block Updates
-Input
-{   "requestor": "andy",   "target": "john@example.com" } </t>
-  </si>
-  <si>
-    <t xml:space="preserve">API 5 - Block Updates
-Input
-{   "requestor": "andy@example.com",   "target": "john" } </t>
-  </si>
-  <si>
-    <t xml:space="preserve">API 6 - Retrieve all email addresses that can receive updates from an email address
-Input
-{   "sender":  "john@example.com",   "text": "Hello World! kate@example.com" } </t>
-  </si>
-  <si>
-    <t xml:space="preserve">API 6 - Retrieve all email addresses that can receive updates from an email address
-Input
-{   "sender":  "john@example.com",   "text": "Hello World!" } </t>
-  </si>
-  <si>
-    <t xml:space="preserve">{   "success": true   "recipients":     [ "lisa@example.com",       "andy@example.com", "common@example.com"   ] } </t>
-  </si>
-  <si>
-    <t xml:space="preserve">{   "success": true   "recipients":     [ "lisa@example.com",       "andy@example.com", "common@example.com", "kate@example.com"    ] } </t>
-  </si>
-  <si>
-    <t>{   "error": Input has to be valid email ID }</t>
+{   "friends":     
+[       "andy@example.com",       "kevin@example.com"     ] } </t>
   </si>
 </sst>
 </file>
@@ -527,7 +527,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA7537E5-3026-44B8-B091-BF86E3931818}">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -558,7 +560,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>5</v>
@@ -569,10 +571,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="58" x14ac:dyDescent="0.35">
@@ -580,7 +582,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>6</v>
@@ -591,7 +593,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>7</v>
@@ -602,7 +604,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>5</v>
@@ -613,7 +615,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>5</v>
@@ -624,10 +626,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="58" x14ac:dyDescent="0.35">
@@ -635,10 +637,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="58" x14ac:dyDescent="0.35">
@@ -646,10 +648,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
@@ -657,10 +659,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
@@ -668,10 +670,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="58" x14ac:dyDescent="0.35">
@@ -679,10 +681,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
@@ -690,10 +692,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
@@ -701,10 +703,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="58" x14ac:dyDescent="0.35">
@@ -712,10 +714,10 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
@@ -723,10 +725,10 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>